<commit_message>
ajout de l'importation de toutes les affectations et terminaison des importations :))))))
</commit_message>
<xml_diff>
--- a/app/Fichiers Excel/GroupePH.xlsx
+++ b/app/Fichiers Excel/GroupePH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yacin\Desktop\eisgi_app\app\Fichiers Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sora7\OneDrive\Desktop\PF SYN\eisgi_app\app\Fichiers Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88332BE3-59EA-4EBD-B822-566124569920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E175B7-FA0C-4AA8-AFCE-0651F06B83A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{963BC95D-5EB6-42D5-AFD0-5305E60F87C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{963BC95D-5EB6-42D5-AFD0-5305E60F87C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
   <si>
     <t>Libellé Groupe</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Gestion des Entreprises Option Ressources Humaines</t>
   </si>
   <si>
-    <t>IDOCS201</t>
-  </si>
-  <si>
     <t>2IDOCS201D1</t>
   </si>
   <si>
@@ -237,6 +234,18 @@
   </si>
   <si>
     <t>Group Physique</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>2IDOCS201</t>
   </si>
 </sst>
 </file>
@@ -613,22 +622,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E491F85-CD29-4C53-92A6-CF6FC3CFF260}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="24.453125" customWidth="1"/>
-    <col min="4" max="4" width="37.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -643,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -656,11 +665,11 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,11 +682,11 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -690,11 +699,11 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -707,11 +716,11 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -724,11 +733,11 @@
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -741,11 +750,11 @@
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -758,11 +767,11 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -775,11 +784,11 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -792,11 +801,11 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -809,11 +818,11 @@
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -826,11 +835,11 @@
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -843,11 +852,11 @@
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -860,11 +869,11 @@
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -877,11 +886,11 @@
       <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -894,11 +903,11 @@
       <c r="D16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -911,11 +920,11 @@
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -928,11 +937,11 @@
       <c r="D18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -945,11 +954,11 @@
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -962,11 +971,11 @@
       <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -979,11 +988,11 @@
       <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -996,11 +1005,11 @@
       <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
@@ -1013,11 +1022,11 @@
       <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1030,11 +1039,11 @@
       <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1047,195 +1056,195 @@
       <c r="D25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E28" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E31" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="1">
-        <v>3</v>
+      <c r="E36" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>